<commit_message>
add dna ids to 144L_2018 datasets
</commit_message>
<xml_diff>
--- a/Input_Data/week3/144L_2018_BactAbund.xlsx
+++ b/Input_Data/week3/144L_2018_BactAbund.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasbaetge/GITHUB/eemb144l/Input_Data/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E29714-1288-D64E-A3EA-5707B41CC0EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38BB174-D4C5-4F42-AC32-372EA7473B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="4300" windowWidth="27640" windowHeight="16940" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView xWindow="11540" yWindow="2280" windowWidth="22500" windowHeight="17720" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="65">
   <si>
     <t>A</t>
   </si>
@@ -154,6 +154,81 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>144_A0_S6</t>
+  </si>
+  <si>
+    <t>144_A4_S7</t>
+  </si>
+  <si>
+    <t>144_A8_S8</t>
+  </si>
+  <si>
+    <t>144_B0_S9</t>
+  </si>
+  <si>
+    <t>144_B4_S10</t>
+  </si>
+  <si>
+    <t>144_B8_S11</t>
+  </si>
+  <si>
+    <t>144_C0_S12</t>
+  </si>
+  <si>
+    <t>144_C4_S13</t>
+  </si>
+  <si>
+    <t>144_C8_S14</t>
+  </si>
+  <si>
+    <t>144_D0_S15</t>
+  </si>
+  <si>
+    <t>144_D4_S16</t>
+  </si>
+  <si>
+    <t>144_D8_S17</t>
+  </si>
+  <si>
+    <t>144_E0_S18</t>
+  </si>
+  <si>
+    <t>144_E4_S19</t>
+  </si>
+  <si>
+    <t>144_E8_S20</t>
+  </si>
+  <si>
+    <t>144_F0_S21</t>
+  </si>
+  <si>
+    <t>144_F4_S22</t>
+  </si>
+  <si>
+    <t>144_F8_S23</t>
+  </si>
+  <si>
+    <t>144_G0_S24</t>
+  </si>
+  <si>
+    <t>144_G4_S25</t>
+  </si>
+  <si>
+    <t>144_G8_S26</t>
+  </si>
+  <si>
+    <t>144_H0_S27</t>
+  </si>
+  <si>
+    <t>144_H4_S28</t>
+  </si>
+  <si>
+    <t>144_H8_S29</t>
+  </si>
+  <si>
+    <t>DNA_SampleID</t>
   </si>
 </sst>
 </file>
@@ -512,15 +587,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB9DCA8-3A58-FF4E-A0AD-EB8E080FD40B}">
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -566,8 +641,11 @@
       <c r="O1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -613,8 +691,11 @@
       <c r="O2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -661,7 +742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -708,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -755,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -801,8 +882,11 @@
       <c r="O6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -849,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -896,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -943,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -989,8 +1073,11 @@
       <c r="O10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1037,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1083,8 +1170,11 @@
       <c r="O12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1178,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1225,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1271,8 +1361,11 @@
       <c r="O16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1366,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1413,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1459,8 +1552,11 @@
       <c r="O20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1507,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1553,8 +1649,11 @@
       <c r="O22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1601,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1648,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1695,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1741,8 +1840,11 @@
       <c r="O26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1789,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1836,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1883,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1929,8 +2031,11 @@
       <c r="O30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1977,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -2023,8 +2128,11 @@
       <c r="O32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -2071,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2118,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -2165,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2211,8 +2319,11 @@
       <c r="O36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -2259,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -2306,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2353,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2399,8 +2510,11 @@
       <c r="O40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -2447,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2493,8 +2607,11 @@
       <c r="O42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -2541,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -2588,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -2635,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -2681,8 +2798,11 @@
       <c r="O46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -2729,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -2776,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -2823,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -2869,8 +2989,11 @@
       <c r="O50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2917,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2963,8 +3086,11 @@
       <c r="O52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -3011,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -3058,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -3105,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3151,8 +3277,11 @@
       <c r="O56" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -3199,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3246,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3293,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3339,8 +3468,11 @@
       <c r="O60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -3387,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -3433,8 +3565,11 @@
       <c r="O62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -3481,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -3528,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -3575,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -3621,8 +3756,11 @@
       <c r="O66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -3669,7 +3807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -3716,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -3763,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -3809,8 +3947,11 @@
       <c r="O70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -3857,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -3903,8 +4044,11 @@
       <c r="O72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P72" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -3951,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -3998,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -4045,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -4091,8 +4235,11 @@
       <c r="O76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -4139,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -4186,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -4233,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -4278,6 +4425,9 @@
       </c>
       <c r="O80" t="b">
         <v>1</v>
+      </c>
+      <c r="P80" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>